<commit_message>
add class 3.1 nomalization
</commit_message>
<xml_diff>
--- a/7-SQL/documents/table-normalization.xlsx
+++ b/7-SQL/documents/table-normalization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/Emanuel/Web-Development-Course/7-SQL/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="8_{1F94925B-2AD6-4DA9-AEBF-FA83BC26E00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBFA278A-F971-45AD-A118-D74F93D6B261}"/>
+  <xr:revisionPtr revIDLastSave="352" documentId="8_{1F94925B-2AD6-4DA9-AEBF-FA83BC26E00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97EDE49A-568B-4624-A2E8-6534F7639C93}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{8C798455-50EB-4E83-8022-F18F926495A9}"/>
   </bookViews>
@@ -385,18 +385,6 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -512,6 +500,18 @@
       </fill>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="8"/>
@@ -592,7 +592,7 @@
     <tableColumn id="4" xr3:uid="{07BA65AB-D573-4710-8F4E-E49C336C7943}" name="STREET"/>
     <tableColumn id="7" xr3:uid="{338F1BCB-288D-49A1-9EEB-A54A2B56CCA7}" name="NEIGHBORHOOD"/>
     <tableColumn id="8" xr3:uid="{21C40E77-E834-4E16-8ABC-8E4517B6764B}" name="CITY"/>
-    <tableColumn id="3" xr3:uid="{D9E0B5D6-16E6-4100-992E-A3CD577CC406}" name="ID_COURSE" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{D9E0B5D6-16E6-4100-992E-A3CD577CC406}" name="ID_COURSE" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{7D819CB7-CA6A-40A8-8979-A89CC6483957}" name="NOME_COURSE"/>
     <tableColumn id="9" xr3:uid="{AF1AFDC6-7FEA-4A8B-9451-D738A036FB14}" name="HOURS"/>
   </tableColumns>
@@ -601,7 +601,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}" name="Tabela2" displayName="Tabela2" ref="J6:S8" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}" name="Tabela2" displayName="Tabela2" ref="J6:S8" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="J6:S8" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{888FD9EF-C11C-496F-B85A-2FCC6B93E363}" name="ID"/>
@@ -620,14 +620,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}" name="Tabela246" displayName="Tabela246" ref="AL6:AQ8" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}" name="Tabela246" displayName="Tabela246" ref="AL6:AQ8" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="AL6:AQ8" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{28F287C0-A642-48A5-BCC1-B0A1A495674E}" name="ID"/>
     <tableColumn id="2" xr3:uid="{36BB37E6-AE69-4E62-A8A3-1A569BD296E9}" name="NAME"/>
     <tableColumn id="4" xr3:uid="{F2B9157B-004C-4384-9E75-7AEFCE9A1DA7}" name="STREET"/>
-    <tableColumn id="7" xr3:uid="{3B8C041B-17AE-4D41-B81A-755AFD2435F0}" name="NEIGHBORHOOD" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{2828DC00-B755-4826-A9A1-6D7D2E127CBC}" name="CITY" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{3B8C041B-17AE-4D41-B81A-755AFD2435F0}" name="NEIGHBORHOOD" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2828DC00-B755-4826-A9A1-6D7D2E127CBC}" name="CITY" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{34CBB47A-217E-40D9-8910-454D24D7B43C}" name="FK_COURSE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -635,7 +635,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}" name="Tabela12" displayName="Tabela12" ref="AD6:AF10" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}" name="Tabela12" displayName="Tabela12" ref="AD6:AF10" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="AD6:AF10" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{78002F2E-C925-48F5-879A-F3CC71F7A559}" name="ID"/>
@@ -647,7 +647,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}" name="Tabela1214" displayName="Tabela1214" ref="AS6:AU10" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}" name="Tabela1214" displayName="Tabela1214" ref="AS6:AU10" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="AS6:AU10" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7EE5BBAB-D493-410D-8287-C04026F1E5D7}" name="ID"/>
@@ -659,7 +659,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}" name="Tabela14" displayName="Tabela14" ref="AH6:AJ8" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}" name="Tabela14" displayName="Tabela14" ref="AH6:AJ8" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="AH6:AJ8" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{9C7382F1-0969-49AC-946F-6BE3B101F2EA}" name="ID"/>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2B1627-A41E-42AA-907F-AFE2A2506E0A}">
   <dimension ref="B3:AU16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:H16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update class 02 components
</commit_message>
<xml_diff>
--- a/7-SQL/documents/table-normalization.xlsx
+++ b/7-SQL/documents/table-normalization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/Emanuel/Web-Development-Course/7-SQL/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="8_{1F94925B-2AD6-4DA9-AEBF-FA83BC26E00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97EDE49A-568B-4624-A2E8-6534F7639C93}"/>
+  <xr:revisionPtr revIDLastSave="367" documentId="8_{1F94925B-2AD6-4DA9-AEBF-FA83BC26E00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CE44A8E-8911-4DF5-9709-9B9F5EF49B82}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{8C798455-50EB-4E83-8022-F18F926495A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
   <si>
     <t>(88)7777-7777, (99) 1234-5678</t>
   </si>
@@ -146,12 +146,6 @@
     <t>Students</t>
   </si>
   <si>
-    <t>PHONE1</t>
-  </si>
-  <si>
-    <t>PHONE2</t>
-  </si>
-  <si>
     <t>0:N</t>
   </si>
   <si>
@@ -165,22 +159,13 @@
   </si>
   <si>
     <t>ID_COURSE</t>
-  </si>
-  <si>
-    <t>ID_SALE</t>
-  </si>
-  <si>
-    <t>DATE_SALE</t>
-  </si>
-  <si>
-    <t>TOTAL_SALE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,16 +217,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,14 +237,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED7D31"/>
-        <bgColor rgb="FFED7D31"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -315,48 +286,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF4B084"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFF4B084"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF4B084"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFF4B084"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF4B084"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFF4B084"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF4B084"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF4B084"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -375,10 +309,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +514,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BB08FAFA-AC36-4225-8885-CE07BE98BA83}" name="Tabela24" displayName="Tabela24" ref="U6:AB8" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="U6:AB8" xr:uid="{BB08FAFA-AC36-4225-8885-CE07BE98BA83}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BB08FAFA-AC36-4225-8885-CE07BE98BA83}" name="Tabela24" displayName="Tabela24" ref="T6:AA8" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="T6:AA8" xr:uid="{BB08FAFA-AC36-4225-8885-CE07BE98BA83}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FC5D0F76-EA8C-4524-97B8-371D897582B0}" name="ID"/>
     <tableColumn id="2" xr3:uid="{C794ADBE-1CF9-4AC2-8699-1281793BE2AD}" name="NAME"/>
@@ -601,13 +531,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}" name="Tabela2" displayName="Tabela2" ref="J6:S8" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="J6:S8" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}" name="Tabela2" displayName="Tabela2" ref="J6:R10" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="J6:R10" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{888FD9EF-C11C-496F-B85A-2FCC6B93E363}" name="ID"/>
     <tableColumn id="2" xr3:uid="{E4F6BA1D-D557-48E7-8DE6-99E68DD8C2EF}" name="NAME"/>
-    <tableColumn id="10" xr3:uid="{F954B888-EE53-4C4D-950C-209BE54C1E00}" name="PHONE1"/>
-    <tableColumn id="3" xr3:uid="{717ABE28-2055-4403-A2E0-35303D973732}" name="PHONE2"/>
+    <tableColumn id="10" xr3:uid="{F954B888-EE53-4C4D-950C-209BE54C1E00}" name="PHONE"/>
     <tableColumn id="4" xr3:uid="{E0B5B222-22C4-4DF0-AADE-9A9B83D8701E}" name="STREET"/>
     <tableColumn id="7" xr3:uid="{98E2317A-8049-46A6-9A8F-ED8E7E39FD9C}" name="NEIGHBORHOOD"/>
     <tableColumn id="8" xr3:uid="{99F67FF7-8B05-48B9-87F2-A695581535B2}" name="CITY"/>
@@ -620,8 +549,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}" name="Tabela246" displayName="Tabela246" ref="AL6:AQ8" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="AL6:AQ8" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}" name="Tabela246" displayName="Tabela246" ref="AK6:AP8" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="AK6:AP8" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{28F287C0-A642-48A5-BCC1-B0A1A495674E}" name="ID"/>
     <tableColumn id="2" xr3:uid="{36BB37E6-AE69-4E62-A8A3-1A569BD296E9}" name="NAME"/>
@@ -635,8 +564,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}" name="Tabela12" displayName="Tabela12" ref="AD6:AF10" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="AD6:AF10" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}" name="Tabela12" displayName="Tabela12" ref="AC6:AE10" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="AC6:AE10" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{78002F2E-C925-48F5-879A-F3CC71F7A559}" name="ID"/>
     <tableColumn id="2" xr3:uid="{2FD2916E-252E-48E7-9A9C-286FD4E707FF}" name="NUMBER"/>
@@ -647,8 +576,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}" name="Tabela1214" displayName="Tabela1214" ref="AS6:AU10" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="AS6:AU10" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}" name="Tabela1214" displayName="Tabela1214" ref="AR6:AT10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="AR6:AT10" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7EE5BBAB-D493-410D-8287-C04026F1E5D7}" name="ID"/>
     <tableColumn id="2" xr3:uid="{6C590E62-773D-4C4D-AA0D-A5DBF949F3FB}" name="NUMBER"/>
@@ -659,30 +588,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}" name="Tabela14" displayName="Tabela14" ref="AH6:AJ8" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="AH6:AJ8" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}" name="Tabela14" displayName="Tabela14" ref="AG6:AI8" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="AG6:AI8" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{9C7382F1-0969-49AC-946F-6BE3B101F2EA}" name="ID"/>
     <tableColumn id="2" xr3:uid="{D7592D99-D1F7-4E04-8ED8-CE0782E0695F}" name="NAME"/>
     <tableColumn id="3" xr3:uid="{50BAE034-7CD2-4979-87A4-F43A93380DB5}" name="HOURS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{10863E4A-865B-4B9B-B4B8-2C4789A5ADF8}" name="Tabela17" displayName="Tabela17" ref="B14:H16" totalsRowShown="0">
-  <autoFilter ref="B14:H16" xr:uid="{10863E4A-865B-4B9B-B4B8-2C4789A5ADF8}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{888137E6-CC2A-497E-83A8-D9CCBA98BA96}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{D39DEF2B-B61F-4BCA-9AEA-D505D8E17DFA}" name="NAME"/>
-    <tableColumn id="3" xr3:uid="{D41ABD69-092B-4550-BD40-30C61E10DB2B}" name="PHONE"/>
-    <tableColumn id="4" xr3:uid="{CF0945A8-08F5-459F-A415-15E1A9D4A9B9}" name="ADDRESS"/>
-    <tableColumn id="5" xr3:uid="{461535AD-F12A-4BE0-86DA-62AD9D2DA5DB}" name="ID_SALE"/>
-    <tableColumn id="6" xr3:uid="{3140A01A-894D-4B1F-A6B9-988F35BE066C}" name="DATE_SALE"/>
-    <tableColumn id="7" xr3:uid="{F4E2E7FF-FD48-4AFD-9584-9095F559BC8C}" name="TOTAL_SALE"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -983,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2B1627-A41E-42AA-907F-AFE2A2506E0A}">
-  <dimension ref="B3:AU16"/>
+  <dimension ref="B3:AT10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1002,112 +915,112 @@
     <col min="9" max="9" width="2.453125" customWidth="1"/>
     <col min="10" max="10" width="4.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:47" ht="21" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:46" ht="21" x14ac:dyDescent="0.5">
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AD3" s="4"/>
-      <c r="AG3" s="4" t="s">
+      <c r="AC3" s="4"/>
+      <c r="AF3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AI3" s="4"/>
-      <c r="AN3" s="4"/>
-      <c r="AS3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AR3" s="4"/>
     </row>
-    <row r="4" spans="2:47" ht="21" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:46" ht="21" x14ac:dyDescent="0.5">
       <c r="C4" s="13" t="s">
         <v>35</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="T4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AD4" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI4" s="4"/>
-      <c r="AN4" s="13" t="s">
+      <c r="AC4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH4" s="4"/>
+      <c r="AM4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AS4" s="13" t="s">
-        <v>39</v>
+      <c r="AR4" s="13" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:47" x14ac:dyDescent="0.35">
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12" t="s">
+    <row r="5" spans="2:46" x14ac:dyDescent="0.35">
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="10" t="s">
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11" t="s">
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AK5" s="10"/>
-      <c r="AL5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP5" s="11"/>
-      <c r="AQ5" s="11" t="s">
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO5" s="11"/>
+      <c r="AP5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AR5" s="10"/>
-      <c r="AS5" s="10" t="s">
-        <v>38</v>
+      <c r="AQ5" s="10"/>
+      <c r="AR5" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="6" spans="2:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1121,7 +1034,7 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -1136,100 +1049,97 @@
         <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="M6" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="N6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V6" t="s">
         <v>18</v>
       </c>
-      <c r="O6" t="s">
+      <c r="W6" t="s">
         <v>19</v>
       </c>
-      <c r="P6" t="s">
+      <c r="X6" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" t="s">
-        <v>42</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="Y6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z6" t="s">
         <v>16</v>
       </c>
-      <c r="S6" t="s">
+      <c r="AA6" t="s">
         <v>17</v>
       </c>
-      <c r="U6" t="s">
+      <c r="AC6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="V6" t="s">
+      <c r="AD6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="W6" t="s">
+      <c r="AI6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="X6" t="s">
+      <c r="AN6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AO6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Z6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AP6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AS6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AT6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AH6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AN6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AO6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="AS6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU6" s="9" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="7" spans="2:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>1</v>
       </c>
@@ -1261,97 +1171,94 @@
         <v>3</v>
       </c>
       <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7">
+        <v>240</v>
+      </c>
+      <c r="T7" s="1">
+        <v>1</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA7">
+        <v>240</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7" t="s">
         <v>4</v>
       </c>
-      <c r="N7" t="s">
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI7">
+        <v>240</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O7" t="s">
+      <c r="AN7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P7" t="s">
+      <c r="AO7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
-        <v>10</v>
-      </c>
-      <c r="S7">
-        <v>240</v>
-      </c>
-      <c r="U7" s="1">
-        <v>1</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB7">
-        <v>240</v>
-      </c>
-      <c r="AD7">
-        <v>1</v>
-      </c>
-      <c r="AE7" t="s">
+      <c r="AP7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AR7">
+        <v>1</v>
+      </c>
+      <c r="AS7" t="s">
         <v>4</v>
       </c>
-      <c r="AF7">
-        <v>1</v>
-      </c>
-      <c r="AH7">
-        <v>1</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ7">
-        <v>240</v>
-      </c>
-      <c r="AL7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AQ7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AS7">
-        <v>1</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AU7">
+      <c r="AT7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>2</v>
       </c>
@@ -1374,219 +1281,201 @@
         <v>160</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8">
+        <v>240</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" t="s">
+        <v>34</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA8">
+        <v>160</v>
+      </c>
+      <c r="AC8">
+        <v>2</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>2</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI8">
+        <v>160</v>
+      </c>
+      <c r="AK8">
+        <v>2</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AR8">
+        <v>2</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:46" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
         <v>9</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R9">
+        <v>160</v>
+      </c>
+      <c r="AC9">
+        <v>3</v>
+      </c>
+      <c r="AD9" t="s">
         <v>8</v>
       </c>
-      <c r="N8" t="s">
+      <c r="AE9">
+        <v>2</v>
+      </c>
+      <c r="AR9">
+        <v>3</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:46" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" t="s">
         <v>34</v>
       </c>
-      <c r="O8" t="s">
+      <c r="N10" t="s">
         <v>29</v>
       </c>
-      <c r="P8" t="s">
+      <c r="O10" t="s">
         <v>30</v>
       </c>
-      <c r="Q8">
-        <v>2</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10" t="s">
         <v>11</v>
       </c>
-      <c r="S8">
+      <c r="R10">
         <v>160</v>
       </c>
-      <c r="U8">
-        <v>2</v>
-      </c>
-      <c r="V8" t="s">
-        <v>2</v>
-      </c>
-      <c r="W8" t="s">
-        <v>34</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB8">
-        <v>160</v>
-      </c>
-      <c r="AD8">
-        <v>2</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF8">
-        <v>1</v>
-      </c>
-      <c r="AH8">
-        <v>2</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ8">
-        <v>160</v>
-      </c>
-      <c r="AL8">
-        <v>2</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AQ8" s="2">
-        <v>2</v>
-      </c>
-      <c r="AS8">
-        <v>2</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>3</v>
-      </c>
-      <c r="AU8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:47" x14ac:dyDescent="0.35">
-      <c r="AD9">
-        <v>3</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF9">
-        <v>2</v>
-      </c>
-      <c r="AS9">
-        <v>3</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:47" x14ac:dyDescent="0.35">
-      <c r="AD10">
+      <c r="AC10">
         <v>4</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AD10" t="s">
         <v>9</v>
       </c>
-      <c r="AF10">
-        <v>2</v>
-      </c>
-      <c r="AS10">
+      <c r="AE10">
+        <v>2</v>
+      </c>
+      <c r="AR10">
         <v>4</v>
       </c>
-      <c r="AT10" t="s">
+      <c r="AS10" t="s">
         <v>9</v>
       </c>
-      <c r="AU10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:47" x14ac:dyDescent="0.35">
-      <c r="B14" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="2:47" x14ac:dyDescent="0.35">
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="17">
-        <v>45351</v>
-      </c>
-      <c r="H15">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="2:47" x14ac:dyDescent="0.35">
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16" s="17">
-        <v>45351</v>
-      </c>
-      <c r="H16">
-        <v>400</v>
+      <c r="AT10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="8">
+  <tableParts count="7">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1594,7 +1483,6 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
-    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update class databases pdf
</commit_message>
<xml_diff>
--- a/7-SQL/documents/table-normalization.xlsx
+++ b/7-SQL/documents/table-normalization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/Emanuel/Web-Development-Course/7-SQL/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="396" documentId="8_{1F94925B-2AD6-4DA9-AEBF-FA83BC26E00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB78237-7505-456B-A5ED-F7A8B8CED33C}"/>
+  <xr:revisionPtr revIDLastSave="414" documentId="8_{1F94925B-2AD6-4DA9-AEBF-FA83BC26E00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97E762FC-1ED4-4302-AEED-7938225D75FF}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{8C798455-50EB-4E83-8022-F18F926495A9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8C798455-50EB-4E83-8022-F18F926495A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="42">
   <si>
     <t>(88)7777-7777, (99) 1234-5678</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Ana</t>
   </si>
   <si>
-    <t>Mario</t>
-  </si>
-  <si>
     <t>(99) 1234-5678</t>
   </si>
   <si>
@@ -158,7 +155,13 @@
     <t>Normalization</t>
   </si>
   <si>
-    <t>ID_COURSE</t>
+    <t>PHONE2</t>
+  </si>
+  <si>
+    <t>PHONE1</t>
+  </si>
+  <si>
+    <t>João</t>
   </si>
 </sst>
 </file>
@@ -313,15 +316,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -438,18 +433,6 @@
       </fill>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="8"/>
@@ -480,6 +463,14 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -493,19 +484,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6433B179-BDC3-4D2F-A14B-6EEE3340F882}" name="Tabela1" displayName="Tabela1" ref="B6:H8" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B6:H8" xr:uid="{6433B179-BDC3-4D2F-A14B-6EEE3340F882}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6433B179-BDC3-4D2F-A14B-6EEE3340F882}" name="Tabela1" displayName="Tabela1" ref="B6:G8" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="B6:G8" xr:uid="{6433B179-BDC3-4D2F-A14B-6EEE3340F882}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{76A83139-FC91-40F7-9D56-2011F6EB95C9}" name="ID"/>
     <tableColumn id="2" xr3:uid="{2249DBB7-77E1-41DA-A8D6-61994346DC8A}" name="NAME"/>
     <tableColumn id="3" xr3:uid="{31C2A5E6-2898-457D-A3DE-0732AFBF77C9}" name="PHONE"/>
     <tableColumn id="4" xr3:uid="{46D97572-3456-43C3-88ED-8662F6B81C6C}" name="ADDRESS"/>
-    <tableColumn id="5" xr3:uid="{19F2609B-2C5A-4CB4-A625-D25B87731A11}" name="ID_COURSE"/>
     <tableColumn id="6" xr3:uid="{DCD2352B-8C9F-4BA0-A3AD-D1B03548E872}" name="NOME_COURSE"/>
     <tableColumn id="7" xr3:uid="{87B69C2D-59C5-4335-9E12-0D24DC9605CA}" name="HOURS"/>
   </tableColumns>
@@ -514,15 +500,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BB08FAFA-AC36-4225-8885-CE07BE98BA83}" name="Tabela24" displayName="Tabela24" ref="T6:AA8" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="T6:AA8" xr:uid="{BB08FAFA-AC36-4225-8885-CE07BE98BA83}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BB08FAFA-AC36-4225-8885-CE07BE98BA83}" name="Tabela24" displayName="Tabela24" ref="S6:Y8" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="S6:Y8" xr:uid="{BB08FAFA-AC36-4225-8885-CE07BE98BA83}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FC5D0F76-EA8C-4524-97B8-371D897582B0}" name="ID"/>
     <tableColumn id="2" xr3:uid="{C794ADBE-1CF9-4AC2-8699-1281793BE2AD}" name="NAME"/>
     <tableColumn id="4" xr3:uid="{07BA65AB-D573-4710-8F4E-E49C336C7943}" name="STREET"/>
     <tableColumn id="7" xr3:uid="{338F1BCB-288D-49A1-9EEB-A54A2B56CCA7}" name="NEIGHBORHOOD"/>
     <tableColumn id="8" xr3:uid="{21C40E77-E834-4E16-8ABC-8E4517B6764B}" name="CITY"/>
-    <tableColumn id="3" xr3:uid="{D9E0B5D6-16E6-4100-992E-A3CD577CC406}" name="ID_COURSE" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{7D819CB7-CA6A-40A8-8979-A89CC6483957}" name="NOME_COURSE"/>
     <tableColumn id="9" xr3:uid="{AF1AFDC6-7FEA-4A8B-9451-D738A036FB14}" name="HOURS"/>
   </tableColumns>
@@ -531,16 +516,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}" name="Tabela2" displayName="Tabela2" ref="J6:R10" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="J6:R10" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}" name="Tabela2" displayName="Tabela2" ref="I6:Q8" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="I6:Q8" xr:uid="{2388B09F-C3B7-4842-B67D-538A61F9765B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{888FD9EF-C11C-496F-B85A-2FCC6B93E363}" name="ID"/>
     <tableColumn id="2" xr3:uid="{E4F6BA1D-D557-48E7-8DE6-99E68DD8C2EF}" name="NAME"/>
-    <tableColumn id="10" xr3:uid="{F954B888-EE53-4C4D-950C-209BE54C1E00}" name="PHONE"/>
+    <tableColumn id="10" xr3:uid="{F954B888-EE53-4C4D-950C-209BE54C1E00}" name="PHONE1"/>
+    <tableColumn id="3" xr3:uid="{4A11DB4A-7AD6-48AE-9999-F81F6B96A05D}" name="PHONE2"/>
     <tableColumn id="4" xr3:uid="{E0B5B222-22C4-4DF0-AADE-9A9B83D8701E}" name="STREET"/>
     <tableColumn id="7" xr3:uid="{98E2317A-8049-46A6-9A8F-ED8E7E39FD9C}" name="NEIGHBORHOOD"/>
     <tableColumn id="8" xr3:uid="{99F67FF7-8B05-48B9-87F2-A695581535B2}" name="CITY"/>
-    <tableColumn id="5" xr3:uid="{B699F8F9-CC84-4ABB-A0FF-C67B94C5109B}" name="ID_COURSE"/>
     <tableColumn id="6" xr3:uid="{DD329CA2-8C99-4140-B404-E17F96EFB7EA}" name="NOME_COURSE"/>
     <tableColumn id="9" xr3:uid="{7AE4E441-6D86-493A-A977-CDC73286F8D9}" name="HOURS"/>
   </tableColumns>
@@ -549,14 +534,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}" name="Tabela246" displayName="Tabela246" ref="AK6:AP8" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="AK6:AP8" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}" name="Tabela246" displayName="Tabela246" ref="AI6:AN8" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="AI6:AN8" xr:uid="{786A556C-FD5F-469D-9939-2F388075F074}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{28F287C0-A642-48A5-BCC1-B0A1A495674E}" name="ID"/>
     <tableColumn id="2" xr3:uid="{36BB37E6-AE69-4E62-A8A3-1A569BD296E9}" name="NAME"/>
     <tableColumn id="4" xr3:uid="{F2B9157B-004C-4384-9E75-7AEFCE9A1DA7}" name="STREET"/>
-    <tableColumn id="7" xr3:uid="{3B8C041B-17AE-4D41-B81A-755AFD2435F0}" name="NEIGHBORHOOD" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{2828DC00-B755-4826-A9A1-6D7D2E127CBC}" name="CITY" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{3B8C041B-17AE-4D41-B81A-755AFD2435F0}" name="NEIGHBORHOOD" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2828DC00-B755-4826-A9A1-6D7D2E127CBC}" name="CITY" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{34CBB47A-217E-40D9-8910-454D24D7B43C}" name="FK_COURSE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -564,8 +549,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}" name="Tabela12" displayName="Tabela12" ref="AC6:AE10" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="AC6:AE10" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}" name="Tabela12" displayName="Tabela12" ref="AA6:AC10" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="AA6:AC10" xr:uid="{C22A364A-D83D-4025-BE8E-90289CF5300B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{78002F2E-C925-48F5-879A-F3CC71F7A559}" name="ID"/>
     <tableColumn id="2" xr3:uid="{2FD2916E-252E-48E7-9A9C-286FD4E707FF}" name="NUMBER"/>
@@ -576,8 +561,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}" name="Tabela1214" displayName="Tabela1214" ref="AR6:AT10" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="AR6:AT10" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}" name="Tabela1214" displayName="Tabela1214" ref="AP6:AR10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="AP6:AR10" xr:uid="{C89930F3-6C9F-4366-8083-0657CF0F69BD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7EE5BBAB-D493-410D-8287-C04026F1E5D7}" name="ID"/>
     <tableColumn id="2" xr3:uid="{6C590E62-773D-4C4D-AA0D-A5DBF949F3FB}" name="NUMBER"/>
@@ -588,8 +573,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}" name="Tabela14" displayName="Tabela14" ref="AG6:AI8" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="AG6:AI8" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}" name="Tabela14" displayName="Tabela14" ref="AE6:AG8" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="AE6:AG8" xr:uid="{F24949A7-706E-4E12-99D7-2BC921C14415}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{9C7382F1-0969-49AC-946F-6BE3B101F2EA}" name="ID"/>
     <tableColumn id="2" xr3:uid="{D7592D99-D1F7-4E04-8ED8-CE0782E0695F}" name="NAME"/>
@@ -896,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2B1627-A41E-42AA-907F-AFE2A2506E0A}">
-  <dimension ref="B3:AT10"/>
+  <dimension ref="B3:AR10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AF1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -909,177 +894,175 @@
     <col min="3" max="3" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.453125" customWidth="1"/>
-    <col min="10" max="10" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.453125" customWidth="1"/>
+    <col min="9" max="9" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:46" ht="21" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:44" ht="21" x14ac:dyDescent="0.5">
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="J3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="4"/>
-      <c r="T3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="S3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="AF3" s="4"/>
-      <c r="AG3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH3" s="4"/>
-      <c r="AM3" s="4"/>
-      <c r="AR3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AP3" s="4"/>
     </row>
-    <row r="4" spans="2:46" ht="21" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:44" ht="21" x14ac:dyDescent="0.5">
       <c r="B4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="I4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="S4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="4"/>
+      <c r="AI4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK4" s="13"/>
+      <c r="AP4" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="J4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="13"/>
-      <c r="T4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH4" s="4"/>
-      <c r="AK4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM4" s="13"/>
-      <c r="AR4" s="13" t="s">
-        <v>37</v>
+      <c r="AM5" s="11"/>
+      <c r="AN5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO5" s="10"/>
+      <c r="AP5" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:46" x14ac:dyDescent="0.35">
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH5" s="11"/>
-      <c r="AI5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO5" s="11"/>
-      <c r="AP5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="AQ5" s="10"/>
-      <c r="AR5" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
-        <v>17</v>
+      <c r="I6" t="s">
+        <v>11</v>
       </c>
       <c r="J6" t="s">
         <v>12</v>
       </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="M6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" t="s">
         <v>18</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>19</v>
       </c>
-      <c r="O6" t="s">
-        <v>20</v>
-      </c>
       <c r="P6" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="Q6" t="s">
         <v>16</v>
       </c>
-      <c r="R6" t="s">
-        <v>17</v>
+      <c r="S6" t="s">
+        <v>11</v>
       </c>
       <c r="T6" t="s">
         <v>12</v>
       </c>
       <c r="U6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="V6" t="s">
         <v>18</v>
@@ -1088,64 +1071,58 @@
         <v>19</v>
       </c>
       <c r="X6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Y6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="AC6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AI6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AC6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AL6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AE6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AK6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AN6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="AP6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="AR6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT6" s="9" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="7" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>1</v>
       </c>
@@ -1156,324 +1133,258 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
         <v>240</v>
       </c>
-      <c r="J7">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" t="s">
         <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" t="s">
         <v>5</v>
       </c>
-      <c r="O7" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>10</v>
-      </c>
-      <c r="R7">
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7">
         <v>240</v>
       </c>
-      <c r="T7" s="1">
+      <c r="S7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="W7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="3" t="s">
-        <v>10</v>
+      <c r="X7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y7">
+        <v>240</v>
       </c>
       <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG7">
         <v>240</v>
       </c>
-      <c r="AC7">
-        <v>1</v>
-      </c>
-      <c r="AD7" t="s">
+      <c r="AI7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AE7">
-        <v>1</v>
-      </c>
-      <c r="AG7">
-        <v>1</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI7">
-        <v>240</v>
-      </c>
-      <c r="AK7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="AM7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AO7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AP7" s="2">
-        <v>1</v>
+      <c r="AN7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AP7">
+        <v>1</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>3</v>
       </c>
       <c r="AR7">
         <v>1</v>
       </c>
-      <c r="AS7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AT7">
-        <v>1</v>
-      </c>
     </row>
-    <row r="8" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>160</v>
+      </c>
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
         <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8">
-        <v>160</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>4</v>
       </c>
       <c r="M8" t="s">
         <v>33</v>
       </c>
       <c r="N8" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="O8" t="s">
-        <v>6</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
         <v>10</v>
       </c>
-      <c r="R8">
-        <v>240</v>
-      </c>
-      <c r="T8">
+      <c r="Q8">
+        <v>160</v>
+      </c>
+      <c r="S8">
         <v>2</v>
       </c>
+      <c r="T8" t="s">
+        <v>41</v>
+      </c>
       <c r="U8" t="s">
-        <v>2</v>
-      </c>
-      <c r="V8" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y8" s="2">
+      <c r="X8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y8">
+        <v>160</v>
+      </c>
+      <c r="AA8">
         <v>2</v>
       </c>
-      <c r="Z8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA8">
+      <c r="AB8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>2</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG8">
         <v>160</v>
       </c>
-      <c r="AC8">
+      <c r="AI8">
         <v>2</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AJ8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AP8">
+        <v>2</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="AA9">
         <v>3</v>
       </c>
-      <c r="AE8">
-        <v>1</v>
-      </c>
-      <c r="AG8">
+      <c r="AB9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC9">
         <v>2</v>
       </c>
-      <c r="AH8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI8">
-        <v>160</v>
-      </c>
-      <c r="AK8">
+      <c r="AP9">
+        <v>3</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR9">
         <v>2</v>
       </c>
-      <c r="AL8" t="s">
+    </row>
+    <row r="10" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="AA10">
+        <v>4</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC10">
         <v>2</v>
       </c>
-      <c r="AM8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AP8" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR8">
-        <v>2</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>3</v>
-      </c>
-      <c r="AT8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:46" x14ac:dyDescent="0.35">
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9">
-        <v>2</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>11</v>
-      </c>
-      <c r="R9">
-        <v>160</v>
-      </c>
-      <c r="AC9">
-        <v>3</v>
-      </c>
-      <c r="AD9" t="s">
+      <c r="AP10">
+        <v>4</v>
+      </c>
+      <c r="AQ10" t="s">
         <v>8</v>
       </c>
-      <c r="AE9">
-        <v>2</v>
-      </c>
-      <c r="AR9">
-        <v>3</v>
-      </c>
-      <c r="AS9" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:46" x14ac:dyDescent="0.35">
-      <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" t="s">
-        <v>29</v>
-      </c>
-      <c r="O10" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10">
-        <v>2</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>11</v>
-      </c>
-      <c r="R10">
-        <v>160</v>
-      </c>
-      <c r="AC10">
-        <v>4</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE10">
-        <v>2</v>
-      </c>
       <c r="AR10">
-        <v>4</v>
-      </c>
-      <c r="AS10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AT10">
         <v>2</v>
       </c>
     </row>

</xml_diff>